<commit_message>
starting assaingment 2 and create visual
</commit_message>
<xml_diff>
--- a/data/betyg_o_prov_riksnivå.xlsx
+++ b/data/betyg_o_prov_riksnivå.xlsx
@@ -4,7 +4,7 @@
   <fileVersion rupBuild="9303" lowestEdited="5" lastEdited="5" appName="xl"/>
   <workbookPr/>
   <bookViews>
-    <workbookView xWindow="480" yWindow="60" windowWidth="18195" windowHeight="8505" activeTab="0"/>
+    <workbookView xWindow="480" yWindow="60" windowWidth="18195" windowHeight="8505" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet r:id="rId1" sheetId="1" name="Tabell 1A"/>
@@ -312,7 +312,7 @@
       <rPr>
         <b/>
         <sz val="10"/>
-        <color theme="1"/>
+        <color rgb="FF000000"/>
         <rFont val="Arial"/>
         <family val="2"/>
       </rPr>
@@ -396,7 +396,7 @@
       <rPr>
         <b/>
         <sz val="10"/>
-        <color theme="1"/>
+        <color rgb="FF000000"/>
         <rFont val="Arial"/>
         <family val="2"/>
       </rPr>
@@ -431,7 +431,7 @@
     <r>
       <rPr>
         <sz val="10"/>
-        <color theme="1"/>
+        <color rgb="FF000000"/>
         <rFont val="Arial"/>
         <family val="2"/>
       </rPr>
@@ -446,7 +446,7 @@
       <rPr>
         <b/>
         <sz val="10"/>
-        <color theme="1"/>
+        <color rgb="FF000000"/>
         <rFont val="Arial"/>
         <family val="2"/>
       </rPr>
@@ -479,19 +479,19 @@
     <font>
       <b/>
       <sz val="12"/>
-      <color theme="1"/>
+      <color rgb="FF000000"/>
       <name val="Arial"/>
       <family val="2"/>
     </font>
     <font>
       <sz val="10"/>
-      <color theme="1"/>
+      <color rgb="FF000000"/>
       <name val="Arial"/>
       <family val="2"/>
     </font>
     <font>
       <sz val="12"/>
-      <color theme="1"/>
+      <color rgb="FF000000"/>
       <name val="Arial"/>
       <family val="2"/>
     </font>
@@ -504,12 +504,6 @@
     </font>
     <font>
       <sz val="9"/>
-      <color theme="1"/>
-      <name val="Arial"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <sz val="10"/>
       <color rgb="FF000000"/>
       <name val="Arial"/>
       <family val="2"/>
@@ -523,35 +517,41 @@
     <font>
       <b/>
       <sz val="10"/>
-      <color theme="1"/>
+      <color rgb="FF000000"/>
       <name val="Arial"/>
       <family val="2"/>
     </font>
     <font>
       <b/>
       <sz val="20"/>
-      <color theme="1"/>
+      <color rgb="FF000000"/>
       <name val="Times New Roman"/>
       <family val="2"/>
     </font>
     <font>
       <b/>
       <sz val="12"/>
-      <color theme="1"/>
+      <color rgb="FF000000"/>
       <name val="Times New Roman"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
       <family val="2"/>
     </font>
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <i/>
-      <sz val="10"/>
-      <color theme="1"/>
-      <name val="Arial"/>
       <family val="2"/>
     </font>
   </fonts>
@@ -782,7 +782,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="101">
+  <cellXfs count="99">
     <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0"/>
     <xf xfId="0" numFmtId="0" borderId="1" applyBorder="1" fontId="1" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -799,15 +799,15 @@
     <xf xfId="0" numFmtId="0" borderId="1" applyBorder="1" fontId="4" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
     <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="2" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf xfId="0" numFmtId="0" borderId="1" applyBorder="1" fontId="5" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf xfId="0" numFmtId="0" borderId="1" applyBorder="1" fontId="6" applyFont="1" fillId="0" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
     <xf xfId="0" numFmtId="4" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="2" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
@@ -826,14 +826,23 @@
     <xf xfId="0" numFmtId="164" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="2" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="7" applyFont="1" fillId="0" applyAlignment="1">
+    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="6" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="left"/>
+    </xf>
+    <xf xfId="0" numFmtId="0" borderId="1" applyBorder="1" fontId="7" applyFont="1" fillId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
+      <alignment horizontal="general"/>
     </xf>
     <xf xfId="0" numFmtId="0" borderId="1" applyBorder="1" fontId="8" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
-      <alignment horizontal="general"/>
+    <xf xfId="0" numFmtId="164" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="8" applyFont="1" fillId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
     <xf xfId="0" numFmtId="0" borderId="1" applyBorder="1" fontId="9" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -841,19 +850,10 @@
     <xf xfId="0" numFmtId="164" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="9" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf xfId="0" numFmtId="164" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="6" applyFont="1" fillId="0" applyAlignment="1">
+    <xf xfId="0" numFmtId="0" borderId="2" applyBorder="1" fontId="10" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf xfId="0" numFmtId="0" borderId="1" applyBorder="1" fontId="10" applyFont="1" fillId="0" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf xfId="0" numFmtId="164" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="10" applyFont="1" fillId="0" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf xfId="0" numFmtId="0" borderId="2" applyBorder="1" fontId="11" applyFont="1" fillId="0" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf xfId="0" numFmtId="164" applyNumberFormat="1" borderId="2" applyBorder="1" fontId="11" applyFont="1" fillId="0" applyAlignment="1">
+    <xf xfId="0" numFmtId="164" applyNumberFormat="1" borderId="2" applyBorder="1" fontId="10" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
@@ -880,52 +880,52 @@
     <xf xfId="0" numFmtId="164" applyNumberFormat="1" borderId="9" applyBorder="1" fontId="2" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf xfId="0" numFmtId="0" borderId="10" applyBorder="1" fontId="8" applyFont="1" fillId="0" applyAlignment="1">
+    <xf xfId="0" numFmtId="0" borderId="10" applyBorder="1" fontId="7" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf xfId="0" numFmtId="164" applyNumberFormat="1" borderId="11" applyBorder="1" fontId="8" applyFont="1" fillId="0" applyAlignment="1">
+    <xf xfId="0" numFmtId="164" applyNumberFormat="1" borderId="11" applyBorder="1" fontId="7" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf xfId="0" numFmtId="164" applyNumberFormat="1" borderId="12" applyBorder="1" fontId="8" applyFont="1" fillId="0" applyAlignment="1">
+    <xf xfId="0" numFmtId="164" applyNumberFormat="1" borderId="12" applyBorder="1" fontId="7" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf xfId="0" numFmtId="164" applyNumberFormat="1" borderId="13" applyBorder="1" fontId="8" applyFont="1" fillId="0" applyAlignment="1">
+    <xf xfId="0" numFmtId="164" applyNumberFormat="1" borderId="13" applyBorder="1" fontId="7" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf xfId="0" numFmtId="164" applyNumberFormat="1" borderId="10" applyBorder="1" fontId="8" applyFont="1" fillId="0" applyAlignment="1">
+    <xf xfId="0" numFmtId="164" applyNumberFormat="1" borderId="10" applyBorder="1" fontId="7" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf xfId="0" numFmtId="164" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="8" applyFont="1" fillId="0" applyAlignment="1">
+    <xf xfId="0" numFmtId="164" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="7" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf xfId="0" numFmtId="164" applyNumberFormat="1" borderId="14" applyBorder="1" fontId="8" applyFont="1" fillId="0" applyAlignment="1">
+    <xf xfId="0" numFmtId="164" applyNumberFormat="1" borderId="14" applyBorder="1" fontId="7" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf xfId="0" numFmtId="0" borderId="15" applyBorder="1" fontId="8" applyFont="1" fillId="0" applyAlignment="1">
+    <xf xfId="0" numFmtId="0" borderId="15" applyBorder="1" fontId="7" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf xfId="0" numFmtId="164" applyNumberFormat="1" borderId="15" applyBorder="1" fontId="8" applyFont="1" fillId="0" applyAlignment="1">
+    <xf xfId="0" numFmtId="164" applyNumberFormat="1" borderId="15" applyBorder="1" fontId="7" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf xfId="0" numFmtId="164" applyNumberFormat="1" borderId="16" applyBorder="1" fontId="8" applyFont="1" fillId="0" applyAlignment="1">
+    <xf xfId="0" numFmtId="164" applyNumberFormat="1" borderId="16" applyBorder="1" fontId="7" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf xfId="0" numFmtId="164" applyNumberFormat="1" borderId="17" applyBorder="1" fontId="8" applyFont="1" fillId="0" applyAlignment="1">
+    <xf xfId="0" numFmtId="164" applyNumberFormat="1" borderId="17" applyBorder="1" fontId="7" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf xfId="0" numFmtId="0" borderId="7" applyBorder="1" fontId="8" applyFont="1" fillId="0" applyAlignment="1">
+    <xf xfId="0" numFmtId="0" borderId="7" applyBorder="1" fontId="7" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf xfId="0" numFmtId="164" applyNumberFormat="1" borderId="10" applyBorder="1" fontId="8" applyFont="1" fillId="0" applyAlignment="1">
+    <xf xfId="0" numFmtId="164" applyNumberFormat="1" borderId="10" applyBorder="1" fontId="7" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="right" wrapText="1"/>
     </xf>
-    <xf xfId="0" numFmtId="164" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="8" applyFont="1" fillId="0" applyAlignment="1">
+    <xf xfId="0" numFmtId="164" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="7" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="right" wrapText="1"/>
     </xf>
-    <xf xfId="0" numFmtId="164" applyNumberFormat="1" borderId="14" applyBorder="1" fontId="8" applyFont="1" fillId="0" applyAlignment="1">
+    <xf xfId="0" numFmtId="164" applyNumberFormat="1" borderId="14" applyBorder="1" fontId="7" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="right" wrapText="1"/>
     </xf>
-    <xf xfId="0" numFmtId="0" borderId="7" applyBorder="1" fontId="12" applyFont="1" fillId="0" applyAlignment="1">
+    <xf xfId="0" numFmtId="0" borderId="7" applyBorder="1" fontId="11" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
     <xf xfId="0" numFmtId="164" applyNumberFormat="1" borderId="10" applyBorder="1" fontId="2" applyFont="1" fillId="0" applyAlignment="1">
@@ -946,28 +946,22 @@
     <xf xfId="0" numFmtId="164" applyNumberFormat="1" borderId="19" applyBorder="1" fontId="2" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="right" wrapText="1"/>
     </xf>
-    <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
     <xf xfId="0" numFmtId="164" applyNumberFormat="1" borderId="0" fontId="0" fillId="0" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf xfId="0" numFmtId="0" borderId="1" applyBorder="1" fontId="9" applyFont="1" fillId="0" applyAlignment="1">
+    <xf xfId="0" numFmtId="0" borderId="1" applyBorder="1" fontId="8" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
+    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="8" applyFont="1" fillId="0" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
     <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="9" applyFont="1" fillId="0" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="6" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="10" applyFont="1" fillId="0" applyAlignment="1">
+    <xf xfId="0" numFmtId="0" borderId="1" applyBorder="1" fontId="12" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="0" fontId="0" fillId="0" applyAlignment="1">
+    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="12" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
     <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="4" applyBorder="1" fontId="2" applyFont="1" fillId="0" applyAlignment="1">
@@ -982,13 +976,13 @@
     <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="3" applyBorder="1" fontId="2" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="4" applyBorder="1" fontId="12" applyFont="1" fillId="0" applyAlignment="1">
+    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="4" applyBorder="1" fontId="11" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="5" applyBorder="1" fontId="12" applyFont="1" fillId="0" applyAlignment="1">
+    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="5" applyBorder="1" fontId="11" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="6" applyBorder="1" fontId="12" applyFont="1" fillId="0" applyAlignment="1">
+    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="6" applyBorder="1" fontId="11" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="7" applyBorder="1" fontId="2" applyFont="1" fillId="0" applyAlignment="1">
@@ -1036,31 +1030,31 @@
     <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="9" applyBorder="1" fontId="2" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="10" applyBorder="1" fontId="8" applyFont="1" fillId="0" applyAlignment="1">
+    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="10" applyBorder="1" fontId="7" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="8" applyFont="1" fillId="0" applyAlignment="1">
+    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="7" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="14" applyBorder="1" fontId="8" applyFont="1" fillId="0" applyAlignment="1">
+    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="14" applyBorder="1" fontId="7" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="15" applyBorder="1" fontId="8" applyFont="1" fillId="0" applyAlignment="1">
+    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="15" applyBorder="1" fontId="7" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="16" applyBorder="1" fontId="8" applyFont="1" fillId="0" applyAlignment="1">
+    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="16" applyBorder="1" fontId="7" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="17" applyBorder="1" fontId="8" applyFont="1" fillId="0" applyAlignment="1">
+    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="17" applyBorder="1" fontId="7" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="10" applyBorder="1" fontId="8" applyFont="1" fillId="0" applyAlignment="1">
+    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="10" applyBorder="1" fontId="7" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="right" wrapText="1"/>
     </xf>
-    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="8" applyFont="1" fillId="0" applyAlignment="1">
+    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="7" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="right" wrapText="1"/>
     </xf>
-    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="14" applyBorder="1" fontId="8" applyFont="1" fillId="0" applyAlignment="1">
+    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="14" applyBorder="1" fontId="7" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="right" wrapText="1"/>
     </xf>
     <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="10" applyBorder="1" fontId="2" applyFont="1" fillId="0" applyAlignment="1">
@@ -1388,175 +1382,175 @@
   </sheetPr>
   <dimension ref="A1:J41"/>
   <sheetViews>
-    <sheetView workbookViewId="0" tabSelected="1"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" style="55" width="38.71928571428572" customWidth="1" bestFit="1"/>
-    <col min="2" max="2" style="100" width="7.2907142857142855" customWidth="1" bestFit="1"/>
-    <col min="3" max="3" style="100" width="7.2907142857142855" customWidth="1" bestFit="1"/>
-    <col min="4" max="4" style="100" width="7.2907142857142855" customWidth="1" bestFit="1"/>
-    <col min="5" max="5" style="100" width="7.2907142857142855" customWidth="1" bestFit="1"/>
-    <col min="6" max="6" style="100" width="7.2907142857142855" customWidth="1" bestFit="1"/>
-    <col min="7" max="7" style="100" width="7.2907142857142855" customWidth="1" bestFit="1"/>
-    <col min="8" max="8" style="100" width="7.2907142857142855" customWidth="1" bestFit="1"/>
-    <col min="9" max="9" style="100" width="7.2907142857142855" customWidth="1" bestFit="1"/>
-    <col min="10" max="10" style="100" width="7.2907142857142855" customWidth="1" bestFit="1"/>
+    <col min="1" max="1" style="17" width="38.71928571428572" customWidth="1" bestFit="1"/>
+    <col min="2" max="2" style="98" width="7.2907142857142855" customWidth="1" bestFit="1"/>
+    <col min="3" max="3" style="98" width="7.2907142857142855" customWidth="1" bestFit="1"/>
+    <col min="4" max="4" style="98" width="7.2907142857142855" customWidth="1" bestFit="1"/>
+    <col min="5" max="5" style="98" width="7.2907142857142855" customWidth="1" bestFit="1"/>
+    <col min="6" max="6" style="98" width="7.2907142857142855" customWidth="1" bestFit="1"/>
+    <col min="7" max="7" style="98" width="7.2907142857142855" customWidth="1" bestFit="1"/>
+    <col min="8" max="8" style="98" width="7.2907142857142855" customWidth="1" bestFit="1"/>
+    <col min="9" max="9" style="98" width="7.2907142857142855" customWidth="1" bestFit="1"/>
+    <col min="10" max="10" style="98" width="7.2907142857142855" customWidth="1" bestFit="1"/>
   </cols>
   <sheetData>
     <row x14ac:dyDescent="0.25" r="1" customHeight="1" ht="21.95" customFormat="1" s="25">
-      <c r="A1" s="57" t="s">
+      <c r="A1" s="56" t="s">
         <v>88</v>
       </c>
-      <c r="B1" s="58"/>
-      <c r="C1" s="58"/>
-      <c r="D1" s="58"/>
-      <c r="E1" s="58"/>
-      <c r="F1" s="58"/>
-      <c r="G1" s="58"/>
-      <c r="H1" s="58"/>
-      <c r="I1" s="58"/>
-      <c r="J1" s="58"/>
+      <c r="B1" s="57"/>
+      <c r="C1" s="57"/>
+      <c r="D1" s="57"/>
+      <c r="E1" s="57"/>
+      <c r="F1" s="57"/>
+      <c r="G1" s="57"/>
+      <c r="H1" s="57"/>
+      <c r="I1" s="57"/>
+      <c r="J1" s="57"/>
     </row>
     <row x14ac:dyDescent="0.25" r="2" customHeight="1" ht="12.75">
-      <c r="A2" s="8" t="s">
+      <c r="A2" s="2" t="s">
         <v>89</v>
       </c>
-      <c r="B2" s="59"/>
-      <c r="C2" s="59"/>
-      <c r="D2" s="59"/>
-      <c r="E2" s="59"/>
-      <c r="F2" s="59"/>
-      <c r="G2" s="59"/>
-      <c r="H2" s="59"/>
-      <c r="I2" s="59"/>
-      <c r="J2" s="59"/>
+      <c r="B2" s="7"/>
+      <c r="C2" s="7"/>
+      <c r="D2" s="7"/>
+      <c r="E2" s="7"/>
+      <c r="F2" s="7"/>
+      <c r="G2" s="7"/>
+      <c r="H2" s="7"/>
+      <c r="I2" s="7"/>
+      <c r="J2" s="7"/>
     </row>
     <row x14ac:dyDescent="0.25" r="3" customHeight="1" ht="12.75">
-      <c r="A3" s="8" t="s">
+      <c r="A3" s="2" t="s">
         <v>89</v>
       </c>
-      <c r="B3" s="59"/>
-      <c r="C3" s="59"/>
-      <c r="D3" s="59"/>
-      <c r="E3" s="59"/>
-      <c r="F3" s="59"/>
-      <c r="G3" s="59"/>
-      <c r="H3" s="59"/>
-      <c r="I3" s="59"/>
-      <c r="J3" s="59"/>
+      <c r="B3" s="7"/>
+      <c r="C3" s="7"/>
+      <c r="D3" s="7"/>
+      <c r="E3" s="7"/>
+      <c r="F3" s="7"/>
+      <c r="G3" s="7"/>
+      <c r="H3" s="7"/>
+      <c r="I3" s="7"/>
+      <c r="J3" s="7"/>
     </row>
     <row x14ac:dyDescent="0.25" r="4" customHeight="1" ht="15">
       <c r="A4" s="21" t="s">
         <v>124</v>
       </c>
-      <c r="B4" s="60"/>
-      <c r="C4" s="60"/>
-      <c r="D4" s="60"/>
-      <c r="E4" s="60"/>
-      <c r="F4" s="60"/>
-      <c r="G4" s="60"/>
-      <c r="H4" s="60"/>
-      <c r="I4" s="60"/>
-      <c r="J4" s="60"/>
+      <c r="B4" s="58"/>
+      <c r="C4" s="58"/>
+      <c r="D4" s="58"/>
+      <c r="E4" s="58"/>
+      <c r="F4" s="58"/>
+      <c r="G4" s="58"/>
+      <c r="H4" s="58"/>
+      <c r="I4" s="58"/>
+      <c r="J4" s="58"/>
     </row>
     <row x14ac:dyDescent="0.25" r="5" customHeight="1" ht="15">
-      <c r="A5" s="61"/>
-      <c r="B5" s="62"/>
-      <c r="C5" s="62"/>
-      <c r="D5" s="62"/>
-      <c r="E5" s="62"/>
-      <c r="F5" s="62"/>
-      <c r="G5" s="62"/>
-      <c r="H5" s="62"/>
-      <c r="I5" s="62"/>
-      <c r="J5" s="62"/>
+      <c r="A5" s="59"/>
+      <c r="B5" s="60"/>
+      <c r="C5" s="60"/>
+      <c r="D5" s="60"/>
+      <c r="E5" s="60"/>
+      <c r="F5" s="60"/>
+      <c r="G5" s="60"/>
+      <c r="H5" s="60"/>
+      <c r="I5" s="60"/>
+      <c r="J5" s="60"/>
     </row>
     <row x14ac:dyDescent="0.25" r="6" customHeight="1" ht="15">
       <c r="A6" s="26" t="s">
         <v>91</v>
       </c>
-      <c r="B6" s="63" t="s">
+      <c r="B6" s="61" t="s">
         <v>125</v>
       </c>
-      <c r="C6" s="64"/>
-      <c r="D6" s="64"/>
-      <c r="E6" s="64"/>
-      <c r="F6" s="64"/>
-      <c r="G6" s="64"/>
-      <c r="H6" s="64"/>
-      <c r="I6" s="64"/>
-      <c r="J6" s="65"/>
+      <c r="C6" s="62"/>
+      <c r="D6" s="62"/>
+      <c r="E6" s="62"/>
+      <c r="F6" s="62"/>
+      <c r="G6" s="62"/>
+      <c r="H6" s="62"/>
+      <c r="I6" s="62"/>
+      <c r="J6" s="63"/>
     </row>
     <row x14ac:dyDescent="0.25" r="7" customHeight="1" ht="15">
       <c r="A7" s="30"/>
-      <c r="B7" s="66" t="s">
+      <c r="B7" s="64" t="s">
         <v>96</v>
       </c>
-      <c r="C7" s="66" t="s">
+      <c r="C7" s="64" t="s">
         <v>97</v>
       </c>
-      <c r="D7" s="66" t="s">
+      <c r="D7" s="64" t="s">
         <v>98</v>
       </c>
-      <c r="E7" s="67" t="s">
+      <c r="E7" s="65" t="s">
         <v>126</v>
       </c>
-      <c r="F7" s="68"/>
-      <c r="G7" s="68"/>
-      <c r="H7" s="68"/>
-      <c r="I7" s="68"/>
-      <c r="J7" s="69"/>
+      <c r="F7" s="66"/>
+      <c r="G7" s="66"/>
+      <c r="H7" s="66"/>
+      <c r="I7" s="66"/>
+      <c r="J7" s="67"/>
     </row>
     <row x14ac:dyDescent="0.25" r="8" customHeight="1" ht="15">
       <c r="A8" s="30"/>
-      <c r="B8" s="70"/>
-      <c r="C8" s="70"/>
-      <c r="D8" s="70"/>
-      <c r="E8" s="71" t="s">
+      <c r="B8" s="68"/>
+      <c r="C8" s="68"/>
+      <c r="D8" s="68"/>
+      <c r="E8" s="69" t="s">
         <v>127</v>
       </c>
-      <c r="F8" s="72"/>
-      <c r="G8" s="73"/>
-      <c r="H8" s="74" t="s">
+      <c r="F8" s="70"/>
+      <c r="G8" s="71"/>
+      <c r="H8" s="72" t="s">
         <v>128</v>
       </c>
-      <c r="I8" s="75"/>
-      <c r="J8" s="76"/>
+      <c r="I8" s="73"/>
+      <c r="J8" s="74"/>
     </row>
     <row x14ac:dyDescent="0.25" r="9" customHeight="1" ht="15">
       <c r="A9" s="30"/>
-      <c r="B9" s="70"/>
-      <c r="C9" s="70"/>
-      <c r="D9" s="70"/>
-      <c r="E9" s="77"/>
-      <c r="F9" s="78"/>
-      <c r="G9" s="79"/>
-      <c r="H9" s="80"/>
-      <c r="I9" s="81"/>
-      <c r="J9" s="82"/>
+      <c r="B9" s="68"/>
+      <c r="C9" s="68"/>
+      <c r="D9" s="68"/>
+      <c r="E9" s="75"/>
+      <c r="F9" s="76"/>
+      <c r="G9" s="77"/>
+      <c r="H9" s="78"/>
+      <c r="I9" s="79"/>
+      <c r="J9" s="80"/>
     </row>
     <row x14ac:dyDescent="0.25" r="10" customHeight="1" ht="15" customFormat="1" s="25">
       <c r="A10" s="31"/>
-      <c r="B10" s="83"/>
-      <c r="C10" s="83"/>
-      <c r="D10" s="83"/>
-      <c r="E10" s="84" t="s">
+      <c r="B10" s="81"/>
+      <c r="C10" s="81"/>
+      <c r="D10" s="81"/>
+      <c r="E10" s="82" t="s">
         <v>96</v>
       </c>
-      <c r="F10" s="84" t="s">
+      <c r="F10" s="82" t="s">
         <v>97</v>
       </c>
-      <c r="G10" s="84" t="s">
+      <c r="G10" s="82" t="s">
         <v>98</v>
       </c>
-      <c r="H10" s="84" t="s">
+      <c r="H10" s="82" t="s">
         <v>96</v>
       </c>
-      <c r="I10" s="84" t="s">
+      <c r="I10" s="82" t="s">
         <v>97</v>
       </c>
-      <c r="J10" s="84" t="s">
+      <c r="J10" s="82" t="s">
         <v>98</v>
       </c>
     </row>
@@ -1564,31 +1558,31 @@
       <c r="A11" s="33" t="s">
         <v>99</v>
       </c>
-      <c r="B11" s="85">
+      <c r="B11" s="83">
         <v>112731</v>
       </c>
-      <c r="C11" s="86">
+      <c r="C11" s="84">
         <v>54667</v>
       </c>
-      <c r="D11" s="87">
+      <c r="D11" s="85">
         <v>58064</v>
       </c>
-      <c r="E11" s="86">
+      <c r="E11" s="84">
         <v>112280</v>
       </c>
-      <c r="F11" s="86">
+      <c r="F11" s="84">
         <v>54430</v>
       </c>
-      <c r="G11" s="86">
+      <c r="G11" s="84">
         <v>57850</v>
       </c>
-      <c r="H11" s="85">
+      <c r="H11" s="83">
         <v>110663</v>
       </c>
-      <c r="I11" s="86">
+      <c r="I11" s="84">
         <v>53757</v>
       </c>
-      <c r="J11" s="87">
+      <c r="J11" s="85">
         <v>56906</v>
       </c>
     </row>
@@ -1596,31 +1590,31 @@
       <c r="A12" s="33" t="s">
         <v>100</v>
       </c>
-      <c r="B12" s="85">
+      <c r="B12" s="83">
         <v>115023</v>
       </c>
-      <c r="C12" s="86">
+      <c r="C12" s="84">
         <v>55670</v>
       </c>
-      <c r="D12" s="87">
+      <c r="D12" s="85">
         <v>59353</v>
       </c>
-      <c r="E12" s="86">
+      <c r="E12" s="84">
         <v>114444</v>
       </c>
-      <c r="F12" s="86">
+      <c r="F12" s="84">
         <v>55389</v>
       </c>
-      <c r="G12" s="86">
+      <c r="G12" s="84">
         <v>59055</v>
       </c>
-      <c r="H12" s="85">
+      <c r="H12" s="83">
         <v>112728</v>
       </c>
-      <c r="I12" s="86">
+      <c r="I12" s="84">
         <v>54711</v>
       </c>
-      <c r="J12" s="87">
+      <c r="J12" s="85">
         <v>58017</v>
       </c>
     </row>
@@ -1628,31 +1622,31 @@
       <c r="A13" s="33" t="s">
         <v>101</v>
       </c>
-      <c r="B13" s="85">
+      <c r="B13" s="83">
         <v>116359</v>
       </c>
-      <c r="C13" s="86">
+      <c r="C13" s="84">
         <v>56715</v>
       </c>
-      <c r="D13" s="87">
+      <c r="D13" s="85">
         <v>59644</v>
       </c>
-      <c r="E13" s="86">
+      <c r="E13" s="84">
         <v>115710</v>
       </c>
-      <c r="F13" s="86">
+      <c r="F13" s="84">
         <v>56394</v>
       </c>
-      <c r="G13" s="86">
+      <c r="G13" s="84">
         <v>59316</v>
       </c>
-      <c r="H13" s="85">
+      <c r="H13" s="83">
         <v>114136</v>
       </c>
-      <c r="I13" s="86">
+      <c r="I13" s="84">
         <v>55721</v>
       </c>
-      <c r="J13" s="87">
+      <c r="J13" s="85">
         <v>58415</v>
       </c>
     </row>
@@ -1660,31 +1654,31 @@
       <c r="A14" s="40" t="s">
         <v>102</v>
       </c>
-      <c r="B14" s="88">
+      <c r="B14" s="86">
         <v>120525</v>
       </c>
-      <c r="C14" s="89">
+      <c r="C14" s="87">
         <v>58513</v>
       </c>
-      <c r="D14" s="90">
+      <c r="D14" s="88">
         <v>62012</v>
       </c>
-      <c r="E14" s="89">
+      <c r="E14" s="87">
         <v>119891</v>
       </c>
-      <c r="F14" s="89">
+      <c r="F14" s="87">
         <v>58207</v>
       </c>
-      <c r="G14" s="89">
+      <c r="G14" s="87">
         <v>61684</v>
       </c>
-      <c r="H14" s="88">
+      <c r="H14" s="86">
         <v>117935</v>
       </c>
-      <c r="I14" s="89">
+      <c r="I14" s="87">
         <v>57312</v>
       </c>
-      <c r="J14" s="90">
+      <c r="J14" s="88">
         <v>60623</v>
       </c>
     </row>
@@ -1692,31 +1686,31 @@
       <c r="A15" s="44" t="s">
         <v>103</v>
       </c>
-      <c r="B15" s="91">
+      <c r="B15" s="89">
         <v>121369</v>
       </c>
-      <c r="C15" s="92">
+      <c r="C15" s="90">
         <v>59043</v>
       </c>
-      <c r="D15" s="93">
+      <c r="D15" s="91">
         <v>62326</v>
       </c>
-      <c r="E15" s="91">
+      <c r="E15" s="89">
         <v>120742</v>
       </c>
-      <c r="F15" s="92">
+      <c r="F15" s="90">
         <v>58703</v>
       </c>
-      <c r="G15" s="93">
+      <c r="G15" s="91">
         <v>62039</v>
       </c>
-      <c r="H15" s="91">
+      <c r="H15" s="89">
         <v>118736</v>
       </c>
-      <c r="I15" s="92">
+      <c r="I15" s="90">
         <v>57781</v>
       </c>
-      <c r="J15" s="93">
+      <c r="J15" s="91">
         <v>60955</v>
       </c>
     </row>
@@ -1724,45 +1718,45 @@
       <c r="A16" s="48" t="s">
         <v>104</v>
       </c>
-      <c r="B16" s="94"/>
-      <c r="C16" s="95"/>
-      <c r="D16" s="96"/>
-      <c r="E16" s="94"/>
-      <c r="F16" s="95"/>
-      <c r="G16" s="96"/>
-      <c r="H16" s="94"/>
-      <c r="I16" s="95"/>
-      <c r="J16" s="96"/>
+      <c r="B16" s="92"/>
+      <c r="C16" s="93"/>
+      <c r="D16" s="94"/>
+      <c r="E16" s="92"/>
+      <c r="F16" s="93"/>
+      <c r="G16" s="94"/>
+      <c r="H16" s="92"/>
+      <c r="I16" s="93"/>
+      <c r="J16" s="94"/>
     </row>
     <row x14ac:dyDescent="0.25" r="17" customHeight="1" ht="15" customFormat="1" s="25">
       <c r="A17" s="30" t="s">
         <v>105</v>
       </c>
-      <c r="B17" s="94">
+      <c r="B17" s="92">
         <v>96204</v>
       </c>
-      <c r="C17" s="95">
+      <c r="C17" s="93">
         <v>46478</v>
       </c>
-      <c r="D17" s="96">
+      <c r="D17" s="94">
         <v>49726</v>
       </c>
-      <c r="E17" s="94">
+      <c r="E17" s="92">
         <v>95991</v>
       </c>
-      <c r="F17" s="95">
+      <c r="F17" s="93">
         <v>46363</v>
       </c>
-      <c r="G17" s="96">
+      <c r="G17" s="94">
         <v>49628</v>
       </c>
-      <c r="H17" s="94">
+      <c r="H17" s="92">
         <v>94276</v>
       </c>
-      <c r="I17" s="95">
+      <c r="I17" s="93">
         <v>45588</v>
       </c>
-      <c r="J17" s="96">
+      <c r="J17" s="94">
         <v>48688</v>
       </c>
     </row>
@@ -1770,45 +1764,45 @@
       <c r="A18" s="48" t="s">
         <v>104</v>
       </c>
-      <c r="B18" s="94"/>
-      <c r="C18" s="95"/>
-      <c r="D18" s="96"/>
-      <c r="E18" s="94"/>
-      <c r="F18" s="95"/>
-      <c r="G18" s="96"/>
-      <c r="H18" s="94"/>
-      <c r="I18" s="95"/>
-      <c r="J18" s="96"/>
+      <c r="B18" s="92"/>
+      <c r="C18" s="93"/>
+      <c r="D18" s="94"/>
+      <c r="E18" s="92"/>
+      <c r="F18" s="93"/>
+      <c r="G18" s="94"/>
+      <c r="H18" s="92"/>
+      <c r="I18" s="93"/>
+      <c r="J18" s="94"/>
     </row>
     <row x14ac:dyDescent="0.25" r="19" customHeight="1" ht="15" customFormat="1" s="25">
       <c r="A19" s="30" t="s">
         <v>129</v>
       </c>
-      <c r="B19" s="94">
+      <c r="B19" s="92">
         <v>213</v>
       </c>
-      <c r="C19" s="95">
+      <c r="C19" s="93">
         <v>115</v>
       </c>
-      <c r="D19" s="96">
+      <c r="D19" s="94">
         <v>98</v>
       </c>
-      <c r="E19" s="94" t="s">
+      <c r="E19" s="92" t="s">
         <v>76</v>
       </c>
-      <c r="F19" s="95" t="s">
+      <c r="F19" s="93" t="s">
         <v>76</v>
       </c>
-      <c r="G19" s="96" t="s">
+      <c r="G19" s="94" t="s">
         <v>76</v>
       </c>
-      <c r="H19" s="94" t="s">
+      <c r="H19" s="92" t="s">
         <v>76</v>
       </c>
-      <c r="I19" s="95" t="s">
+      <c r="I19" s="93" t="s">
         <v>76</v>
       </c>
-      <c r="J19" s="96" t="s">
+      <c r="J19" s="94" t="s">
         <v>76</v>
       </c>
     </row>
@@ -1816,31 +1810,31 @@
       <c r="A20" s="30" t="s">
         <v>106</v>
       </c>
-      <c r="B20" s="94">
+      <c r="B20" s="92">
         <v>25165</v>
       </c>
-      <c r="C20" s="95">
+      <c r="C20" s="93">
         <v>12565</v>
       </c>
-      <c r="D20" s="96">
+      <c r="D20" s="94">
         <v>12600</v>
       </c>
-      <c r="E20" s="94">
+      <c r="E20" s="92">
         <v>24751</v>
       </c>
-      <c r="F20" s="95">
+      <c r="F20" s="93">
         <v>12340</v>
       </c>
-      <c r="G20" s="96">
+      <c r="G20" s="94">
         <v>12411</v>
       </c>
-      <c r="H20" s="94">
+      <c r="H20" s="92">
         <v>24460</v>
       </c>
-      <c r="I20" s="95">
+      <c r="I20" s="93">
         <v>12193</v>
       </c>
-      <c r="J20" s="96">
+      <c r="J20" s="94">
         <v>12267</v>
       </c>
     </row>
@@ -1848,45 +1842,45 @@
       <c r="A21" s="48" t="s">
         <v>104</v>
       </c>
-      <c r="B21" s="94"/>
-      <c r="C21" s="95"/>
-      <c r="D21" s="96"/>
-      <c r="E21" s="94"/>
-      <c r="F21" s="95"/>
-      <c r="G21" s="96"/>
-      <c r="H21" s="94"/>
-      <c r="I21" s="95"/>
-      <c r="J21" s="96"/>
+      <c r="B21" s="92"/>
+      <c r="C21" s="93"/>
+      <c r="D21" s="94"/>
+      <c r="E21" s="92"/>
+      <c r="F21" s="93"/>
+      <c r="G21" s="94"/>
+      <c r="H21" s="92"/>
+      <c r="I21" s="93"/>
+      <c r="J21" s="94"/>
     </row>
     <row x14ac:dyDescent="0.25" r="22" customHeight="1" ht="15" customFormat="1" s="25">
       <c r="A22" s="30" t="s">
         <v>107</v>
       </c>
-      <c r="B22" s="94">
+      <c r="B22" s="92">
         <v>23085</v>
       </c>
-      <c r="C22" s="95">
+      <c r="C22" s="93">
         <v>11511</v>
       </c>
-      <c r="D22" s="96">
+      <c r="D22" s="94">
         <v>11574</v>
       </c>
-      <c r="E22" s="94">
+      <c r="E22" s="92">
         <v>23085</v>
       </c>
-      <c r="F22" s="95">
+      <c r="F22" s="93">
         <v>11511</v>
       </c>
-      <c r="G22" s="96">
+      <c r="G22" s="94">
         <v>11574</v>
       </c>
-      <c r="H22" s="94">
+      <c r="H22" s="92">
         <v>22815</v>
       </c>
-      <c r="I22" s="95">
+      <c r="I22" s="93">
         <v>11372</v>
       </c>
-      <c r="J22" s="96">
+      <c r="J22" s="94">
         <v>11443</v>
       </c>
     </row>
@@ -1894,31 +1888,31 @@
       <c r="A23" s="30" t="s">
         <v>108</v>
       </c>
-      <c r="B23" s="94">
+      <c r="B23" s="92">
         <v>1036</v>
       </c>
-      <c r="C23" s="95">
+      <c r="C23" s="93">
         <v>532</v>
       </c>
-      <c r="D23" s="96">
+      <c r="D23" s="94">
         <v>504</v>
       </c>
-      <c r="E23" s="94">
+      <c r="E23" s="92">
         <v>1036</v>
       </c>
-      <c r="F23" s="95">
+      <c r="F23" s="93">
         <v>532</v>
       </c>
-      <c r="G23" s="96">
+      <c r="G23" s="94">
         <v>504</v>
       </c>
-      <c r="H23" s="94">
+      <c r="H23" s="92">
         <v>1025</v>
       </c>
-      <c r="I23" s="95">
+      <c r="I23" s="93">
         <v>526</v>
       </c>
-      <c r="J23" s="96">
+      <c r="J23" s="94">
         <v>499</v>
       </c>
     </row>
@@ -1926,31 +1920,31 @@
       <c r="A24" s="30" t="s">
         <v>109</v>
       </c>
-      <c r="B24" s="94">
+      <c r="B24" s="92">
         <v>630</v>
       </c>
-      <c r="C24" s="95">
+      <c r="C24" s="93">
         <v>297</v>
       </c>
-      <c r="D24" s="96">
+      <c r="D24" s="94">
         <v>333</v>
       </c>
-      <c r="E24" s="94">
+      <c r="E24" s="92">
         <v>630</v>
       </c>
-      <c r="F24" s="95">
+      <c r="F24" s="93">
         <v>297</v>
       </c>
-      <c r="G24" s="96">
+      <c r="G24" s="94">
         <v>333</v>
       </c>
-      <c r="H24" s="94">
+      <c r="H24" s="92">
         <v>620</v>
       </c>
-      <c r="I24" s="95">
+      <c r="I24" s="93">
         <v>295</v>
       </c>
-      <c r="J24" s="96">
+      <c r="J24" s="94">
         <v>325</v>
       </c>
     </row>
@@ -1958,31 +1952,31 @@
       <c r="A25" s="30" t="s">
         <v>129</v>
       </c>
-      <c r="B25" s="94">
+      <c r="B25" s="92">
         <v>414</v>
       </c>
-      <c r="C25" s="95">
+      <c r="C25" s="93">
         <v>225</v>
       </c>
-      <c r="D25" s="96">
+      <c r="D25" s="94">
         <v>189</v>
       </c>
-      <c r="E25" s="94" t="s">
+      <c r="E25" s="92" t="s">
         <v>76</v>
       </c>
-      <c r="F25" s="95" t="s">
+      <c r="F25" s="93" t="s">
         <v>76</v>
       </c>
-      <c r="G25" s="96" t="s">
+      <c r="G25" s="94" t="s">
         <v>76</v>
       </c>
-      <c r="H25" s="94" t="s">
+      <c r="H25" s="92" t="s">
         <v>76</v>
       </c>
-      <c r="I25" s="95" t="s">
+      <c r="I25" s="93" t="s">
         <v>76</v>
       </c>
-      <c r="J25" s="96" t="s">
+      <c r="J25" s="94" t="s">
         <v>76</v>
       </c>
     </row>
@@ -1990,31 +1984,31 @@
       <c r="A26" s="30" t="s">
         <v>110</v>
       </c>
-      <c r="B26" s="94">
+      <c r="B26" s="92">
         <v>88383</v>
       </c>
-      <c r="C26" s="95">
+      <c r="C26" s="93">
         <v>43044</v>
       </c>
-      <c r="D26" s="96">
+      <c r="D26" s="94">
         <v>45339</v>
       </c>
-      <c r="E26" s="94">
+      <c r="E26" s="92">
         <v>88214</v>
       </c>
-      <c r="F26" s="95">
+      <c r="F26" s="93">
         <v>42961</v>
       </c>
-      <c r="G26" s="96">
+      <c r="G26" s="94">
         <v>45253</v>
       </c>
-      <c r="H26" s="94">
+      <c r="H26" s="92">
         <v>86799</v>
       </c>
-      <c r="I26" s="95">
+      <c r="I26" s="93">
         <v>42274</v>
       </c>
-      <c r="J26" s="96">
+      <c r="J26" s="94">
         <v>44525</v>
       </c>
     </row>
@@ -2022,31 +2016,31 @@
       <c r="A27" s="30" t="s">
         <v>111</v>
       </c>
-      <c r="B27" s="94">
+      <c r="B27" s="92">
         <v>31918</v>
       </c>
-      <c r="C27" s="95">
+      <c r="C27" s="93">
         <v>15488</v>
       </c>
-      <c r="D27" s="96">
+      <c r="D27" s="94">
         <v>16430</v>
       </c>
-      <c r="E27" s="94">
+      <c r="E27" s="92">
         <v>31488</v>
       </c>
-      <c r="F27" s="95">
+      <c r="F27" s="93">
         <v>15247</v>
       </c>
-      <c r="G27" s="96">
+      <c r="G27" s="94">
         <v>16241</v>
       </c>
-      <c r="H27" s="94">
+      <c r="H27" s="92">
         <v>30999</v>
       </c>
-      <c r="I27" s="95">
+      <c r="I27" s="93">
         <v>15066</v>
       </c>
-      <c r="J27" s="96">
+      <c r="J27" s="94">
         <v>15933</v>
       </c>
     </row>
@@ -2054,45 +2048,45 @@
       <c r="A28" s="48" t="s">
         <v>104</v>
       </c>
-      <c r="B28" s="94"/>
-      <c r="C28" s="95"/>
-      <c r="D28" s="96"/>
-      <c r="E28" s="94"/>
-      <c r="F28" s="95"/>
-      <c r="G28" s="96"/>
-      <c r="H28" s="94"/>
-      <c r="I28" s="95"/>
-      <c r="J28" s="96"/>
+      <c r="B28" s="92"/>
+      <c r="C28" s="93"/>
+      <c r="D28" s="94"/>
+      <c r="E28" s="92"/>
+      <c r="F28" s="93"/>
+      <c r="G28" s="94"/>
+      <c r="H28" s="92"/>
+      <c r="I28" s="93"/>
+      <c r="J28" s="94"/>
     </row>
     <row x14ac:dyDescent="0.25" r="29" customHeight="1" ht="15" customFormat="1" s="25">
       <c r="A29" s="30" t="s">
         <v>112</v>
       </c>
-      <c r="B29" s="94">
+      <c r="B29" s="92">
         <v>13927</v>
       </c>
-      <c r="C29" s="95">
+      <c r="C29" s="93">
         <v>6831</v>
       </c>
-      <c r="D29" s="96">
+      <c r="D29" s="94">
         <v>7096</v>
       </c>
-      <c r="E29" s="94">
+      <c r="E29" s="92">
         <v>13876</v>
       </c>
-      <c r="F29" s="95">
+      <c r="F29" s="93">
         <v>6807</v>
       </c>
-      <c r="G29" s="96">
+      <c r="G29" s="94">
         <v>7069</v>
       </c>
-      <c r="H29" s="94">
+      <c r="H29" s="92">
         <v>13709</v>
       </c>
-      <c r="I29" s="95">
+      <c r="I29" s="93">
         <v>6735</v>
       </c>
-      <c r="J29" s="96">
+      <c r="J29" s="94">
         <v>6974</v>
       </c>
     </row>
@@ -2100,31 +2094,31 @@
       <c r="A30" s="30" t="s">
         <v>113</v>
       </c>
-      <c r="B30" s="94">
+      <c r="B30" s="92">
         <v>6431</v>
       </c>
-      <c r="C30" s="95">
+      <c r="C30" s="93">
         <v>3078</v>
       </c>
-      <c r="D30" s="96">
+      <c r="D30" s="94">
         <v>3353</v>
       </c>
-      <c r="E30" s="94">
+      <c r="E30" s="92">
         <v>6340</v>
       </c>
-      <c r="F30" s="95">
+      <c r="F30" s="93">
         <v>3025</v>
       </c>
-      <c r="G30" s="96">
+      <c r="G30" s="94">
         <v>3315</v>
       </c>
-      <c r="H30" s="94">
+      <c r="H30" s="92">
         <v>6269</v>
       </c>
-      <c r="I30" s="95">
+      <c r="I30" s="93">
         <v>2993</v>
       </c>
-      <c r="J30" s="96">
+      <c r="J30" s="94">
         <v>3276</v>
       </c>
     </row>
@@ -2132,31 +2126,31 @@
       <c r="A31" s="30" t="s">
         <v>114</v>
       </c>
-      <c r="B31" s="94">
+      <c r="B31" s="92">
         <v>11560</v>
       </c>
-      <c r="C31" s="95">
+      <c r="C31" s="93">
         <v>5579</v>
       </c>
-      <c r="D31" s="96">
+      <c r="D31" s="94">
         <v>5981</v>
       </c>
-      <c r="E31" s="94">
+      <c r="E31" s="92">
         <v>11272</v>
       </c>
-      <c r="F31" s="95">
+      <c r="F31" s="93">
         <v>5415</v>
       </c>
-      <c r="G31" s="96">
+      <c r="G31" s="94">
         <v>5857</v>
       </c>
-      <c r="H31" s="94">
+      <c r="H31" s="92">
         <v>11021</v>
       </c>
-      <c r="I31" s="95">
+      <c r="I31" s="93">
         <v>5338</v>
       </c>
-      <c r="J31" s="96">
+      <c r="J31" s="94">
         <v>5683</v>
       </c>
     </row>
@@ -2164,31 +2158,31 @@
       <c r="A32" s="30" t="s">
         <v>115</v>
       </c>
-      <c r="B32" s="94">
+      <c r="B32" s="92">
         <v>117503</v>
       </c>
-      <c r="C32" s="95">
+      <c r="C32" s="93">
         <v>57195</v>
       </c>
-      <c r="D32" s="96">
+      <c r="D32" s="94">
         <v>60308</v>
       </c>
-      <c r="E32" s="94">
+      <c r="E32" s="92">
         <v>117044</v>
       </c>
-      <c r="F32" s="95">
+      <c r="F32" s="93">
         <v>56952</v>
       </c>
-      <c r="G32" s="96">
+      <c r="G32" s="94">
         <v>60092</v>
       </c>
-      <c r="H32" s="94">
+      <c r="H32" s="92">
         <v>115254</v>
       </c>
-      <c r="I32" s="95">
+      <c r="I32" s="93">
         <v>56114</v>
       </c>
-      <c r="J32" s="96">
+      <c r="J32" s="94">
         <v>59140</v>
       </c>
     </row>
@@ -2196,31 +2190,31 @@
       <c r="A33" s="30" t="s">
         <v>116</v>
       </c>
-      <c r="B33" s="94">
+      <c r="B33" s="92">
         <v>2799</v>
       </c>
-      <c r="C33" s="95">
+      <c r="C33" s="93">
         <v>1338</v>
       </c>
-      <c r="D33" s="96">
+      <c r="D33" s="94">
         <v>1461</v>
       </c>
-      <c r="E33" s="94">
+      <c r="E33" s="92">
         <v>2658</v>
       </c>
-      <c r="F33" s="95">
+      <c r="F33" s="93">
         <v>1256</v>
       </c>
-      <c r="G33" s="96">
+      <c r="G33" s="94">
         <v>1402</v>
       </c>
-      <c r="H33" s="94">
+      <c r="H33" s="92">
         <v>2544</v>
       </c>
-      <c r="I33" s="95">
+      <c r="I33" s="93">
         <v>1226</v>
       </c>
-      <c r="J33" s="96">
+      <c r="J33" s="94">
         <v>1318</v>
       </c>
     </row>
@@ -2228,31 +2222,31 @@
       <c r="A34" s="30" t="s">
         <v>117</v>
       </c>
-      <c r="B34" s="94">
+      <c r="B34" s="92">
         <v>1067</v>
       </c>
-      <c r="C34" s="95">
+      <c r="C34" s="93">
         <v>510</v>
       </c>
-      <c r="D34" s="96">
+      <c r="D34" s="94">
         <v>557</v>
       </c>
-      <c r="E34" s="94">
+      <c r="E34" s="92">
         <v>1040</v>
       </c>
-      <c r="F34" s="95">
+      <c r="F34" s="93">
         <v>495</v>
       </c>
-      <c r="G34" s="96">
+      <c r="G34" s="94">
         <v>545</v>
       </c>
-      <c r="H34" s="94">
+      <c r="H34" s="92">
         <v>938</v>
       </c>
-      <c r="I34" s="95">
+      <c r="I34" s="93">
         <v>441</v>
       </c>
-      <c r="J34" s="96">
+      <c r="J34" s="94">
         <v>497</v>
       </c>
     </row>
@@ -2260,45 +2254,45 @@
       <c r="A35" s="30" t="s">
         <v>118</v>
       </c>
-      <c r="B35" s="94"/>
-      <c r="C35" s="95"/>
-      <c r="D35" s="96"/>
-      <c r="E35" s="94"/>
-      <c r="F35" s="95"/>
-      <c r="G35" s="96"/>
-      <c r="H35" s="94"/>
-      <c r="I35" s="95"/>
-      <c r="J35" s="96"/>
+      <c r="B35" s="92"/>
+      <c r="C35" s="93"/>
+      <c r="D35" s="94"/>
+      <c r="E35" s="92"/>
+      <c r="F35" s="93"/>
+      <c r="G35" s="94"/>
+      <c r="H35" s="92"/>
+      <c r="I35" s="93"/>
+      <c r="J35" s="94"/>
     </row>
     <row x14ac:dyDescent="0.25" r="36" customHeight="1" ht="15" customFormat="1" s="25">
       <c r="A36" s="30" t="s">
         <v>119</v>
       </c>
-      <c r="B36" s="94">
+      <c r="B36" s="92">
         <v>6578</v>
       </c>
-      <c r="C36" s="95">
+      <c r="C36" s="93">
         <v>3197</v>
       </c>
-      <c r="D36" s="96">
+      <c r="D36" s="94">
         <v>3381</v>
       </c>
-      <c r="E36" s="94">
+      <c r="E36" s="92">
         <v>6575</v>
       </c>
-      <c r="F36" s="95">
+      <c r="F36" s="93">
         <v>3197</v>
       </c>
-      <c r="G36" s="96">
+      <c r="G36" s="94">
         <v>3378</v>
       </c>
-      <c r="H36" s="94">
+      <c r="H36" s="92">
         <v>6327</v>
       </c>
-      <c r="I36" s="95">
+      <c r="I36" s="93">
         <v>3091</v>
       </c>
-      <c r="J36" s="96">
+      <c r="J36" s="94">
         <v>3236</v>
       </c>
     </row>
@@ -2306,31 +2300,31 @@
       <c r="A37" s="30" t="s">
         <v>120</v>
       </c>
-      <c r="B37" s="94">
+      <c r="B37" s="92">
         <v>36842</v>
       </c>
-      <c r="C37" s="95">
+      <c r="C37" s="93">
         <v>17909</v>
       </c>
-      <c r="D37" s="96">
+      <c r="D37" s="94">
         <v>18933</v>
       </c>
-      <c r="E37" s="94">
+      <c r="E37" s="92">
         <v>36810</v>
       </c>
-      <c r="F37" s="95">
+      <c r="F37" s="93">
         <v>17893</v>
       </c>
-      <c r="G37" s="96">
+      <c r="G37" s="94">
         <v>18917</v>
       </c>
-      <c r="H37" s="94">
+      <c r="H37" s="92">
         <v>35938</v>
       </c>
-      <c r="I37" s="95">
+      <c r="I37" s="93">
         <v>17488</v>
       </c>
-      <c r="J37" s="96">
+      <c r="J37" s="94">
         <v>18450</v>
       </c>
     </row>
@@ -2338,31 +2332,31 @@
       <c r="A38" s="30" t="s">
         <v>121</v>
       </c>
-      <c r="B38" s="94">
+      <c r="B38" s="92">
         <v>74793</v>
       </c>
-      <c r="C38" s="95">
+      <c r="C38" s="93">
         <v>36473</v>
       </c>
-      <c r="D38" s="96">
+      <c r="D38" s="94">
         <v>38320</v>
       </c>
-      <c r="E38" s="94">
+      <c r="E38" s="92">
         <v>74283</v>
       </c>
-      <c r="F38" s="95">
+      <c r="F38" s="93">
         <v>36201</v>
       </c>
-      <c r="G38" s="96">
+      <c r="G38" s="94">
         <v>38082</v>
       </c>
-      <c r="H38" s="94">
+      <c r="H38" s="92">
         <v>73583</v>
       </c>
-      <c r="I38" s="95">
+      <c r="I38" s="93">
         <v>35871</v>
       </c>
-      <c r="J38" s="96">
+      <c r="J38" s="94">
         <v>37712</v>
       </c>
     </row>
@@ -2370,45 +2364,45 @@
       <c r="A39" s="48" t="s">
         <v>104</v>
       </c>
-      <c r="B39" s="94"/>
-      <c r="C39" s="95"/>
-      <c r="D39" s="96"/>
-      <c r="E39" s="94"/>
-      <c r="F39" s="95"/>
-      <c r="G39" s="96"/>
-      <c r="H39" s="94"/>
-      <c r="I39" s="95"/>
-      <c r="J39" s="96"/>
+      <c r="B39" s="92"/>
+      <c r="C39" s="93"/>
+      <c r="D39" s="94"/>
+      <c r="E39" s="92"/>
+      <c r="F39" s="93"/>
+      <c r="G39" s="94"/>
+      <c r="H39" s="92"/>
+      <c r="I39" s="93"/>
+      <c r="J39" s="94"/>
     </row>
     <row x14ac:dyDescent="0.25" r="40" customHeight="1" ht="15" customFormat="1" s="25">
       <c r="A40" s="30" t="s">
         <v>122</v>
       </c>
-      <c r="B40" s="94">
+      <c r="B40" s="92">
         <v>18682</v>
       </c>
-      <c r="C40" s="95">
+      <c r="C40" s="93">
         <v>9215</v>
       </c>
-      <c r="D40" s="96">
+      <c r="D40" s="94">
         <v>9467</v>
       </c>
-      <c r="E40" s="94">
+      <c r="E40" s="92">
         <v>18628</v>
       </c>
-      <c r="F40" s="95">
+      <c r="F40" s="93">
         <v>9189</v>
       </c>
-      <c r="G40" s="96">
+      <c r="G40" s="94">
         <v>9439</v>
       </c>
-      <c r="H40" s="94">
+      <c r="H40" s="92">
         <v>18384</v>
       </c>
-      <c r="I40" s="95">
+      <c r="I40" s="93">
         <v>9073</v>
       </c>
-      <c r="J40" s="96">
+      <c r="J40" s="94">
         <v>9311</v>
       </c>
     </row>
@@ -2416,31 +2410,31 @@
       <c r="A41" s="31" t="s">
         <v>123</v>
       </c>
-      <c r="B41" s="97">
+      <c r="B41" s="95">
         <v>56111</v>
       </c>
-      <c r="C41" s="98">
+      <c r="C41" s="96">
         <v>27258</v>
       </c>
-      <c r="D41" s="99">
+      <c r="D41" s="97">
         <v>28853</v>
       </c>
-      <c r="E41" s="97">
+      <c r="E41" s="95">
         <v>55655</v>
       </c>
-      <c r="F41" s="98">
+      <c r="F41" s="96">
         <v>27012</v>
       </c>
-      <c r="G41" s="99">
+      <c r="G41" s="97">
         <v>28643</v>
       </c>
-      <c r="H41" s="97">
+      <c r="H41" s="95">
         <v>55199</v>
       </c>
-      <c r="I41" s="98">
+      <c r="I41" s="96">
         <v>26798</v>
       </c>
-      <c r="J41" s="99">
+      <c r="J41" s="97">
         <v>28401</v>
       </c>
     </row>
@@ -2471,63 +2465,63 @@
   </sheetPr>
   <dimension ref="A1:J36"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0" tabSelected="1"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" style="55" width="38.71928571428572" customWidth="1" bestFit="1"/>
-    <col min="2" max="2" style="56" width="7.2907142857142855" customWidth="1" bestFit="1"/>
-    <col min="3" max="3" style="56" width="7.2907142857142855" customWidth="1" bestFit="1"/>
-    <col min="4" max="4" style="56" width="7.2907142857142855" customWidth="1" bestFit="1"/>
-    <col min="5" max="5" style="56" width="7.2907142857142855" customWidth="1" bestFit="1"/>
-    <col min="6" max="6" style="56" width="7.2907142857142855" customWidth="1" bestFit="1"/>
-    <col min="7" max="7" style="56" width="7.2907142857142855" customWidth="1" bestFit="1"/>
-    <col min="8" max="8" style="56" width="7.2907142857142855" customWidth="1" bestFit="1"/>
-    <col min="9" max="9" style="56" width="7.2907142857142855" customWidth="1" bestFit="1"/>
-    <col min="10" max="10" style="56" width="7.2907142857142855" customWidth="1" bestFit="1"/>
+    <col min="1" max="1" style="17" width="38.71928571428572" customWidth="1" bestFit="1"/>
+    <col min="2" max="2" style="55" width="7.2907142857142855" customWidth="1" bestFit="1"/>
+    <col min="3" max="3" style="55" width="7.2907142857142855" customWidth="1" bestFit="1"/>
+    <col min="4" max="4" style="55" width="7.2907142857142855" customWidth="1" bestFit="1"/>
+    <col min="5" max="5" style="55" width="7.2907142857142855" customWidth="1" bestFit="1"/>
+    <col min="6" max="6" style="55" width="7.2907142857142855" customWidth="1" bestFit="1"/>
+    <col min="7" max="7" style="55" width="7.2907142857142855" customWidth="1" bestFit="1"/>
+    <col min="8" max="8" style="55" width="7.2907142857142855" customWidth="1" bestFit="1"/>
+    <col min="9" max="9" style="55" width="7.2907142857142855" customWidth="1" bestFit="1"/>
+    <col min="10" max="10" style="55" width="7.2907142857142855" customWidth="1" bestFit="1"/>
   </cols>
   <sheetData>
     <row x14ac:dyDescent="0.25" r="1" customHeight="1" ht="29.25">
-      <c r="A1" s="18" t="s">
+      <c r="A1" s="19" t="s">
         <v>88</v>
       </c>
-      <c r="B1" s="19"/>
-      <c r="C1" s="19"/>
-      <c r="D1" s="19"/>
-      <c r="E1" s="19"/>
-      <c r="F1" s="19"/>
-      <c r="G1" s="19"/>
-      <c r="H1" s="19"/>
-      <c r="I1" s="19"/>
-      <c r="J1" s="19"/>
+      <c r="B1" s="20"/>
+      <c r="C1" s="20"/>
+      <c r="D1" s="20"/>
+      <c r="E1" s="20"/>
+      <c r="F1" s="20"/>
+      <c r="G1" s="20"/>
+      <c r="H1" s="20"/>
+      <c r="I1" s="20"/>
+      <c r="J1" s="20"/>
     </row>
     <row x14ac:dyDescent="0.25" r="2" customHeight="1" ht="18.75">
-      <c r="A2" s="8" t="s">
+      <c r="A2" s="2" t="s">
         <v>89</v>
       </c>
-      <c r="B2" s="20"/>
-      <c r="C2" s="20"/>
-      <c r="D2" s="20"/>
-      <c r="E2" s="20"/>
-      <c r="F2" s="20"/>
-      <c r="G2" s="20"/>
-      <c r="H2" s="20"/>
-      <c r="I2" s="20"/>
-      <c r="J2" s="20"/>
+      <c r="B2" s="14"/>
+      <c r="C2" s="14"/>
+      <c r="D2" s="14"/>
+      <c r="E2" s="14"/>
+      <c r="F2" s="14"/>
+      <c r="G2" s="14"/>
+      <c r="H2" s="14"/>
+      <c r="I2" s="14"/>
+      <c r="J2" s="14"/>
     </row>
     <row x14ac:dyDescent="0.25" r="3" customHeight="1" ht="18.75">
-      <c r="A3" s="8" t="s">
+      <c r="A3" s="2" t="s">
         <v>89</v>
       </c>
-      <c r="B3" s="20"/>
-      <c r="C3" s="20"/>
-      <c r="D3" s="20"/>
-      <c r="E3" s="20"/>
-      <c r="F3" s="20"/>
-      <c r="G3" s="20"/>
-      <c r="H3" s="20"/>
-      <c r="I3" s="20"/>
-      <c r="J3" s="20"/>
+      <c r="B3" s="14"/>
+      <c r="C3" s="14"/>
+      <c r="D3" s="14"/>
+      <c r="E3" s="14"/>
+      <c r="F3" s="14"/>
+      <c r="G3" s="14"/>
+      <c r="H3" s="14"/>
+      <c r="I3" s="14"/>
+      <c r="J3" s="14"/>
     </row>
     <row x14ac:dyDescent="0.25" r="4" customHeight="1" ht="19.5">
       <c r="A4" s="21" t="s">
@@ -3251,7 +3245,7 @@
       <c r="I30" s="50"/>
       <c r="J30" s="51"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="31" customHeight="1" ht="15" customFormat="1" s="25">
+    <row x14ac:dyDescent="0.25" r="31" customHeight="1" ht="18.75" customFormat="1" s="25">
       <c r="A31" s="30" t="s">
         <v>119</v>
       </c>
@@ -3283,7 +3277,7 @@
         <v>65.3</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="32" customHeight="1" ht="15" customFormat="1" s="25">
+    <row x14ac:dyDescent="0.25" r="32" customHeight="1" ht="18.75" customFormat="1" s="25">
       <c r="A32" s="30" t="s">
         <v>120</v>
       </c>
@@ -3315,7 +3309,7 @@
         <v>39.5</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="33" customHeight="1" ht="15" customFormat="1" s="25">
+    <row x14ac:dyDescent="0.25" r="33" customHeight="1" ht="18.75" customFormat="1" s="25">
       <c r="A33" s="30" t="s">
         <v>121</v>
       </c>
@@ -3347,7 +3341,7 @@
         <v>17.5</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="34" customHeight="1" ht="15" customFormat="1" s="25">
+    <row x14ac:dyDescent="0.25" r="34" customHeight="1" ht="18.75" customFormat="1" s="25">
       <c r="A34" s="48" t="s">
         <v>104</v>
       </c>
@@ -3361,7 +3355,7 @@
       <c r="I34" s="50"/>
       <c r="J34" s="51"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="35" customHeight="1" ht="15" customFormat="1" s="25">
+    <row x14ac:dyDescent="0.25" r="35" customHeight="1" ht="18.75" customFormat="1" s="25">
       <c r="A35" s="30" t="s">
         <v>122</v>
       </c>
@@ -3393,7 +3387,7 @@
         <v>27.5</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="36" customHeight="1" ht="15" customFormat="1" s="25">
+    <row x14ac:dyDescent="0.25" r="36" customHeight="1" ht="18.75" customFormat="1" s="25">
       <c r="A36" s="31" t="s">
         <v>123</v>
       </c>
@@ -3456,18 +3450,18 @@
     <col min="1" max="1" style="17" width="3.1478571428571427" customWidth="1" bestFit="1"/>
     <col min="2" max="2" style="17" width="9.147857142857141" customWidth="1" bestFit="1"/>
     <col min="3" max="3" style="17" width="9.147857142857141" customWidth="1" bestFit="1"/>
-    <col min="4" max="4" style="17" width="9.147857142857141" customWidth="1" bestFit="1"/>
+    <col min="4" max="4" style="18" width="9.147857142857141" customWidth="1" bestFit="1"/>
     <col min="5" max="5" style="17" width="8.290714285714287" customWidth="1" bestFit="1"/>
     <col min="6" max="6" style="17" width="9.147857142857141" customWidth="1" bestFit="1"/>
-    <col min="7" max="7" style="17" width="9.147857142857141" customWidth="1" bestFit="1"/>
+    <col min="7" max="7" style="18" width="9.147857142857141" customWidth="1" bestFit="1"/>
     <col min="8" max="8" style="17" width="13.576428571428572" customWidth="1" bestFit="1"/>
     <col min="9" max="9" style="17" width="13.576428571428572" customWidth="1" bestFit="1"/>
     <col min="10" max="10" style="17" width="13.576428571428572" customWidth="1" bestFit="1"/>
     <col min="11" max="11" style="17" width="13.576428571428572" customWidth="1" bestFit="1"/>
     <col min="12" max="12" style="17" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="13" max="13" style="17" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="14" max="14" style="17" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="15" max="15" style="17" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="13" max="13" style="18" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="14" max="14" style="18" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="15" max="15" style="18" width="13.576428571428572" customWidth="1" bestFit="1"/>
   </cols>
   <sheetData>
     <row x14ac:dyDescent="0.25" r="1" customHeight="1" ht="18.75">
@@ -3484,24 +3478,24 @@
       <c r="I1" s="4"/>
       <c r="J1" s="4"/>
       <c r="K1" s="4"/>
-      <c r="L1" s="3"/>
+      <c r="L1" s="6"/>
       <c r="M1" s="3"/>
       <c r="N1" s="3"/>
       <c r="O1" s="3"/>
     </row>
     <row x14ac:dyDescent="0.25" r="2" customHeight="1" ht="18.75">
-      <c r="A2" s="6"/>
+      <c r="A2" s="7"/>
       <c r="B2" s="2"/>
       <c r="C2" s="2"/>
       <c r="D2" s="3"/>
-      <c r="E2" s="7"/>
+      <c r="E2" s="8"/>
       <c r="F2" s="2"/>
       <c r="G2" s="3"/>
-      <c r="H2" s="7"/>
-      <c r="I2" s="7"/>
-      <c r="J2" s="7"/>
-      <c r="K2" s="7"/>
-      <c r="L2" s="3"/>
+      <c r="H2" s="8"/>
+      <c r="I2" s="8"/>
+      <c r="J2" s="8"/>
+      <c r="K2" s="8"/>
+      <c r="L2" s="6"/>
       <c r="M2" s="3"/>
       <c r="N2" s="3"/>
       <c r="O2" s="3"/>
@@ -3547,7 +3541,7 @@
       <c r="O4" s="3"/>
     </row>
     <row x14ac:dyDescent="0.25" r="5" customHeight="1" ht="18.75">
-      <c r="A5" s="6"/>
+      <c r="A5" s="7"/>
       <c r="B5" s="2"/>
       <c r="C5" s="2"/>
       <c r="D5" s="3"/>
@@ -3566,7 +3560,7 @@
       <c r="O5" s="3"/>
     </row>
     <row x14ac:dyDescent="0.25" r="6" customHeight="1" ht="18.75">
-      <c r="A6" s="6"/>
+      <c r="A6" s="7"/>
       <c r="B6" s="2"/>
       <c r="C6" s="2"/>
       <c r="D6" s="3"/>
@@ -3579,13 +3573,13 @@
       <c r="I6" s="2"/>
       <c r="J6" s="2"/>
       <c r="K6" s="2"/>
-      <c r="L6" s="8"/>
+      <c r="L6" s="2"/>
       <c r="M6" s="3"/>
       <c r="N6" s="3"/>
       <c r="O6" s="3"/>
     </row>
     <row x14ac:dyDescent="0.25" r="7" customHeight="1" ht="18.75">
-      <c r="A7" s="6"/>
+      <c r="A7" s="7"/>
       <c r="B7" s="2"/>
       <c r="C7" s="2"/>
       <c r="D7" s="3"/>
@@ -3596,7 +3590,7 @@
       <c r="I7" s="2"/>
       <c r="J7" s="2"/>
       <c r="K7" s="2"/>
-      <c r="L7" s="8"/>
+      <c r="L7" s="2"/>
       <c r="M7" s="3"/>
       <c r="N7" s="3"/>
       <c r="O7" s="3"/>
@@ -3606,9 +3600,9 @@
         <v>6</v>
       </c>
       <c r="B8" s="2"/>
-      <c r="C8" s="6"/>
+      <c r="C8" s="7"/>
       <c r="D8" s="3"/>
-      <c r="E8" s="6"/>
+      <c r="E8" s="7"/>
       <c r="F8" s="2" t="s">
         <v>7</v>
       </c>
@@ -3623,11 +3617,11 @@
       <c r="O8" s="3"/>
     </row>
     <row x14ac:dyDescent="0.25" r="9" customHeight="1" ht="18.75">
-      <c r="A9" s="6"/>
+      <c r="A9" s="7"/>
       <c r="B9" s="2"/>
-      <c r="C9" s="6"/>
+      <c r="C9" s="7"/>
       <c r="D9" s="3"/>
-      <c r="E9" s="6"/>
+      <c r="E9" s="7"/>
       <c r="F9" s="2" t="s">
         <v>8</v>
       </c>
@@ -3642,12 +3636,12 @@
       <c r="O9" s="3"/>
     </row>
     <row x14ac:dyDescent="0.25" r="10" customHeight="1" ht="18.75">
-      <c r="A10" s="6"/>
+      <c r="A10" s="7"/>
       <c r="B10" s="2"/>
-      <c r="C10" s="6"/>
+      <c r="C10" s="7"/>
       <c r="D10" s="3"/>
-      <c r="E10" s="6"/>
-      <c r="F10" s="6"/>
+      <c r="E10" s="7"/>
+      <c r="F10" s="7"/>
       <c r="G10" s="3"/>
       <c r="H10" s="2"/>
       <c r="I10" s="2"/>
@@ -3663,9 +3657,9 @@
         <v>9</v>
       </c>
       <c r="B11" s="2"/>
-      <c r="C11" s="6"/>
+      <c r="C11" s="7"/>
       <c r="D11" s="3"/>
-      <c r="E11" s="6"/>
+      <c r="E11" s="7"/>
       <c r="F11" s="2" t="s">
         <v>10</v>
       </c>
@@ -3684,9 +3678,9 @@
         <v>11</v>
       </c>
       <c r="B12" s="2"/>
-      <c r="C12" s="6"/>
+      <c r="C12" s="7"/>
       <c r="D12" s="3"/>
-      <c r="E12" s="6"/>
+      <c r="E12" s="7"/>
       <c r="F12" s="2" t="s">
         <v>12</v>
       </c>
@@ -3701,12 +3695,12 @@
       <c r="O12" s="3"/>
     </row>
     <row x14ac:dyDescent="0.25" r="13" customHeight="1" ht="18.75">
-      <c r="A13" s="6"/>
+      <c r="A13" s="7"/>
       <c r="B13" s="2"/>
-      <c r="C13" s="6"/>
+      <c r="C13" s="7"/>
       <c r="D13" s="3"/>
-      <c r="E13" s="6"/>
-      <c r="F13" s="6"/>
+      <c r="E13" s="7"/>
+      <c r="F13" s="7"/>
       <c r="G13" s="3"/>
       <c r="H13" s="2"/>
       <c r="I13" s="2"/>
@@ -3967,7 +3961,7 @@
       <c r="O26" s="3"/>
     </row>
     <row x14ac:dyDescent="0.25" r="27" customHeight="1" ht="18.75">
-      <c r="A27" s="6"/>
+      <c r="A27" s="7"/>
       <c r="B27" s="2"/>
       <c r="C27" s="10"/>
       <c r="D27" s="3"/>
@@ -3988,9 +3982,9 @@
     <row x14ac:dyDescent="0.25" r="28" customHeight="1" ht="18.75">
       <c r="A28" s="2"/>
       <c r="B28" s="2"/>
-      <c r="C28" s="6"/>
+      <c r="C28" s="7"/>
       <c r="D28" s="3"/>
-      <c r="E28" s="6"/>
+      <c r="E28" s="7"/>
       <c r="F28" s="2" t="s">
         <v>28</v>
       </c>
@@ -4007,10 +4001,10 @@
     <row x14ac:dyDescent="0.25" r="29" customHeight="1" ht="18.75">
       <c r="A29" s="2"/>
       <c r="B29" s="2"/>
-      <c r="C29" s="6"/>
+      <c r="C29" s="7"/>
       <c r="D29" s="3"/>
-      <c r="E29" s="6"/>
-      <c r="F29" s="6"/>
+      <c r="E29" s="7"/>
+      <c r="F29" s="7"/>
       <c r="G29" s="3"/>
       <c r="H29" s="2"/>
       <c r="I29" s="2"/>
@@ -4026,9 +4020,9 @@
         <v>29</v>
       </c>
       <c r="B30" s="2"/>
-      <c r="C30" s="6"/>
+      <c r="C30" s="7"/>
       <c r="D30" s="3"/>
-      <c r="E30" s="6"/>
+      <c r="E30" s="7"/>
       <c r="F30" s="2" t="s">
         <v>30</v>
       </c>
@@ -4045,9 +4039,9 @@
     <row x14ac:dyDescent="0.25" r="31" customHeight="1" ht="18.75">
       <c r="A31" s="2"/>
       <c r="B31" s="2"/>
-      <c r="C31" s="6"/>
+      <c r="C31" s="7"/>
       <c r="D31" s="3"/>
-      <c r="E31" s="6"/>
+      <c r="E31" s="7"/>
       <c r="F31" s="2" t="s">
         <v>31</v>
       </c>
@@ -4064,9 +4058,9 @@
     <row x14ac:dyDescent="0.25" r="32" customHeight="1" ht="18.75">
       <c r="A32" s="2"/>
       <c r="B32" s="2"/>
-      <c r="C32" s="6"/>
+      <c r="C32" s="7"/>
       <c r="D32" s="3"/>
-      <c r="E32" s="6"/>
+      <c r="E32" s="7"/>
       <c r="F32" s="2" t="s">
         <v>32</v>
       </c>
@@ -4083,18 +4077,18 @@
     <row x14ac:dyDescent="0.25" r="33" customHeight="1" ht="18.75">
       <c r="A33" s="2"/>
       <c r="B33" s="2"/>
-      <c r="C33" s="6"/>
+      <c r="C33" s="7"/>
       <c r="D33" s="3"/>
-      <c r="E33" s="6"/>
+      <c r="E33" s="7"/>
       <c r="F33" s="2" t="s">
         <v>33</v>
       </c>
       <c r="G33" s="3"/>
-      <c r="H33" s="6"/>
-      <c r="I33" s="6"/>
-      <c r="J33" s="6"/>
-      <c r="K33" s="6"/>
-      <c r="L33" s="6"/>
+      <c r="H33" s="7"/>
+      <c r="I33" s="7"/>
+      <c r="J33" s="7"/>
+      <c r="K33" s="7"/>
+      <c r="L33" s="7"/>
       <c r="M33" s="3"/>
       <c r="N33" s="3"/>
       <c r="O33" s="3"/>
@@ -4102,18 +4096,18 @@
     <row x14ac:dyDescent="0.25" r="34" customHeight="1" ht="18.75">
       <c r="A34" s="2"/>
       <c r="B34" s="2"/>
-      <c r="C34" s="6"/>
+      <c r="C34" s="7"/>
       <c r="D34" s="3"/>
-      <c r="E34" s="6"/>
+      <c r="E34" s="7"/>
       <c r="F34" s="2" t="s">
         <v>34</v>
       </c>
       <c r="G34" s="3"/>
-      <c r="H34" s="6"/>
-      <c r="I34" s="6"/>
-      <c r="J34" s="6"/>
-      <c r="K34" s="6"/>
-      <c r="L34" s="6"/>
+      <c r="H34" s="7"/>
+      <c r="I34" s="7"/>
+      <c r="J34" s="7"/>
+      <c r="K34" s="7"/>
+      <c r="L34" s="7"/>
       <c r="M34" s="3"/>
       <c r="N34" s="3"/>
       <c r="O34" s="3"/>
@@ -4121,47 +4115,47 @@
     <row x14ac:dyDescent="0.25" r="35" customHeight="1" ht="18.75">
       <c r="A35" s="2"/>
       <c r="B35" s="2"/>
-      <c r="C35" s="6"/>
+      <c r="C35" s="7"/>
       <c r="D35" s="3"/>
-      <c r="E35" s="6"/>
+      <c r="E35" s="7"/>
       <c r="F35" s="2" t="s">
         <v>35</v>
       </c>
       <c r="G35" s="3"/>
-      <c r="H35" s="6"/>
-      <c r="I35" s="6"/>
-      <c r="J35" s="6"/>
-      <c r="K35" s="6"/>
-      <c r="L35" s="6"/>
-      <c r="M35" s="6"/>
-      <c r="N35" s="6"/>
-      <c r="O35" s="6"/>
+      <c r="H35" s="7"/>
+      <c r="I35" s="7"/>
+      <c r="J35" s="7"/>
+      <c r="K35" s="7"/>
+      <c r="L35" s="7"/>
+      <c r="M35" s="7"/>
+      <c r="N35" s="7"/>
+      <c r="O35" s="7"/>
     </row>
     <row x14ac:dyDescent="0.25" r="36" customHeight="1" ht="18.75">
       <c r="A36" s="2"/>
       <c r="B36" s="2"/>
-      <c r="C36" s="6"/>
+      <c r="C36" s="7"/>
       <c r="D36" s="3"/>
-      <c r="E36" s="6"/>
-      <c r="F36" s="6"/>
+      <c r="E36" s="7"/>
+      <c r="F36" s="7"/>
       <c r="G36" s="3"/>
       <c r="H36" s="2"/>
       <c r="I36" s="2"/>
       <c r="J36" s="2"/>
       <c r="K36" s="2"/>
       <c r="L36" s="2"/>
-      <c r="M36" s="6"/>
-      <c r="N36" s="6"/>
-      <c r="O36" s="6"/>
+      <c r="M36" s="7"/>
+      <c r="N36" s="7"/>
+      <c r="O36" s="7"/>
     </row>
     <row x14ac:dyDescent="0.25" r="37" customHeight="1" ht="18.75">
       <c r="A37" s="2" t="s">
         <v>36</v>
       </c>
       <c r="B37" s="2"/>
-      <c r="C37" s="6"/>
+      <c r="C37" s="7"/>
       <c r="D37" s="3"/>
-      <c r="E37" s="6"/>
+      <c r="E37" s="7"/>
       <c r="F37" s="2" t="s">
         <v>37</v>
       </c>
@@ -4171,16 +4165,16 @@
       <c r="J37" s="2"/>
       <c r="K37" s="2"/>
       <c r="L37" s="2"/>
-      <c r="M37" s="6"/>
-      <c r="N37" s="6"/>
-      <c r="O37" s="6"/>
+      <c r="M37" s="7"/>
+      <c r="N37" s="7"/>
+      <c r="O37" s="7"/>
     </row>
     <row x14ac:dyDescent="0.25" r="38" customHeight="1" ht="18.75">
-      <c r="A38" s="6"/>
+      <c r="A38" s="7"/>
       <c r="B38" s="2"/>
-      <c r="C38" s="6"/>
+      <c r="C38" s="7"/>
       <c r="D38" s="3"/>
-      <c r="E38" s="6"/>
+      <c r="E38" s="7"/>
       <c r="F38" s="2" t="s">
         <v>38</v>
       </c>
@@ -4195,12 +4189,12 @@
       <c r="O38" s="3"/>
     </row>
     <row x14ac:dyDescent="0.25" r="39" customHeight="1" ht="18.75">
-      <c r="A39" s="6"/>
+      <c r="A39" s="7"/>
       <c r="B39" s="2"/>
-      <c r="C39" s="6"/>
+      <c r="C39" s="7"/>
       <c r="D39" s="3"/>
-      <c r="E39" s="6"/>
-      <c r="F39" s="6"/>
+      <c r="E39" s="7"/>
+      <c r="F39" s="7"/>
       <c r="G39" s="3"/>
       <c r="H39" s="2"/>
       <c r="I39" s="2"/>
@@ -4216,9 +4210,9 @@
         <v>36</v>
       </c>
       <c r="B40" s="2"/>
-      <c r="C40" s="6"/>
+      <c r="C40" s="7"/>
       <c r="D40" s="3"/>
-      <c r="E40" s="6"/>
+      <c r="E40" s="7"/>
       <c r="F40" s="2" t="s">
         <v>39</v>
       </c>
@@ -4237,10 +4231,10 @@
         <v>40</v>
       </c>
       <c r="B41" s="2"/>
-      <c r="C41" s="6"/>
+      <c r="C41" s="7"/>
       <c r="D41" s="3"/>
-      <c r="E41" s="6"/>
-      <c r="F41" s="6"/>
+      <c r="E41" s="7"/>
+      <c r="F41" s="7"/>
       <c r="G41" s="3"/>
       <c r="H41" s="2"/>
       <c r="I41" s="2"/>
@@ -4252,12 +4246,12 @@
       <c r="O41" s="3"/>
     </row>
     <row x14ac:dyDescent="0.25" r="42" customHeight="1" ht="18.75">
-      <c r="A42" s="6"/>
+      <c r="A42" s="7"/>
       <c r="B42" s="2"/>
-      <c r="C42" s="6"/>
+      <c r="C42" s="7"/>
       <c r="D42" s="3"/>
-      <c r="E42" s="6"/>
-      <c r="F42" s="6"/>
+      <c r="E42" s="7"/>
+      <c r="F42" s="7"/>
       <c r="G42" s="3"/>
       <c r="H42" s="2"/>
       <c r="I42" s="2"/>
@@ -4273,9 +4267,9 @@
         <v>41</v>
       </c>
       <c r="B43" s="2"/>
-      <c r="C43" s="6"/>
+      <c r="C43" s="7"/>
       <c r="D43" s="3"/>
-      <c r="E43" s="6"/>
+      <c r="E43" s="7"/>
       <c r="F43" s="2" t="s">
         <v>42</v>
       </c>
@@ -4294,9 +4288,9 @@
         <v>43</v>
       </c>
       <c r="B44" s="2"/>
-      <c r="C44" s="6"/>
+      <c r="C44" s="7"/>
       <c r="D44" s="3"/>
-      <c r="E44" s="6"/>
+      <c r="E44" s="7"/>
       <c r="F44" s="2" t="s">
         <v>44</v>
       </c>
@@ -4311,12 +4305,12 @@
       <c r="O44" s="3"/>
     </row>
     <row x14ac:dyDescent="0.25" r="45" customHeight="1" ht="18.75">
-      <c r="A45" s="6"/>
+      <c r="A45" s="7"/>
       <c r="B45" s="2"/>
-      <c r="C45" s="6"/>
+      <c r="C45" s="7"/>
       <c r="D45" s="3"/>
-      <c r="E45" s="6"/>
-      <c r="F45" s="6"/>
+      <c r="E45" s="7"/>
+      <c r="F45" s="7"/>
       <c r="G45" s="3"/>
       <c r="H45" s="2"/>
       <c r="I45" s="2"/>
@@ -4332,9 +4326,9 @@
         <v>41</v>
       </c>
       <c r="B46" s="2"/>
-      <c r="C46" s="6"/>
+      <c r="C46" s="7"/>
       <c r="D46" s="3"/>
-      <c r="E46" s="6"/>
+      <c r="E46" s="7"/>
       <c r="F46" s="2" t="s">
         <v>45</v>
       </c>
@@ -4353,9 +4347,9 @@
         <v>46</v>
       </c>
       <c r="B47" s="2"/>
-      <c r="C47" s="6"/>
+      <c r="C47" s="7"/>
       <c r="D47" s="3"/>
-      <c r="E47" s="6"/>
+      <c r="E47" s="7"/>
       <c r="F47" s="2" t="s">
         <v>47</v>
       </c>
@@ -4370,12 +4364,12 @@
       <c r="O47" s="3"/>
     </row>
     <row x14ac:dyDescent="0.25" r="48" customHeight="1" ht="18.75">
-      <c r="A48" s="6"/>
+      <c r="A48" s="7"/>
       <c r="B48" s="2"/>
-      <c r="C48" s="6"/>
+      <c r="C48" s="7"/>
       <c r="D48" s="3"/>
-      <c r="E48" s="6"/>
-      <c r="F48" s="6"/>
+      <c r="E48" s="7"/>
+      <c r="F48" s="7"/>
       <c r="G48" s="3"/>
       <c r="H48" s="2"/>
       <c r="I48" s="2"/>
@@ -4391,9 +4385,9 @@
         <v>48</v>
       </c>
       <c r="B49" s="2"/>
-      <c r="C49" s="6"/>
+      <c r="C49" s="7"/>
       <c r="D49" s="3"/>
-      <c r="E49" s="6"/>
+      <c r="E49" s="7"/>
       <c r="F49" s="2" t="s">
         <v>49</v>
       </c>
@@ -4412,9 +4406,9 @@
         <v>50</v>
       </c>
       <c r="B50" s="2"/>
-      <c r="C50" s="6"/>
+      <c r="C50" s="7"/>
       <c r="D50" s="3"/>
-      <c r="E50" s="6"/>
+      <c r="E50" s="7"/>
       <c r="F50" s="2" t="s">
         <v>51</v>
       </c>
@@ -4431,10 +4425,10 @@
     <row x14ac:dyDescent="0.25" r="51" customHeight="1" ht="18.75">
       <c r="A51" s="15"/>
       <c r="B51" s="2"/>
-      <c r="C51" s="6"/>
+      <c r="C51" s="7"/>
       <c r="D51" s="3"/>
-      <c r="E51" s="6"/>
-      <c r="F51" s="6"/>
+      <c r="E51" s="7"/>
+      <c r="F51" s="7"/>
       <c r="G51" s="3"/>
       <c r="H51" s="2"/>
       <c r="I51" s="2"/>
@@ -4450,9 +4444,9 @@
         <v>52</v>
       </c>
       <c r="B52" s="2"/>
-      <c r="C52" s="6"/>
+      <c r="C52" s="7"/>
       <c r="D52" s="3"/>
-      <c r="E52" s="6"/>
+      <c r="E52" s="7"/>
       <c r="F52" s="2" t="s">
         <v>53</v>
       </c>
@@ -4467,11 +4461,11 @@
       <c r="O52" s="3"/>
     </row>
     <row x14ac:dyDescent="0.25" r="53" customHeight="1" ht="18.75">
-      <c r="A53" s="6"/>
+      <c r="A53" s="7"/>
       <c r="B53" s="2"/>
-      <c r="C53" s="6"/>
+      <c r="C53" s="7"/>
       <c r="D53" s="3"/>
-      <c r="E53" s="6"/>
+      <c r="E53" s="7"/>
       <c r="F53" s="2" t="s">
         <v>54</v>
       </c>
@@ -4486,12 +4480,12 @@
       <c r="O53" s="3"/>
     </row>
     <row x14ac:dyDescent="0.25" r="54" customHeight="1" ht="18.75">
-      <c r="A54" s="6"/>
+      <c r="A54" s="7"/>
       <c r="B54" s="2"/>
-      <c r="C54" s="6"/>
+      <c r="C54" s="7"/>
       <c r="D54" s="3"/>
-      <c r="E54" s="6"/>
-      <c r="F54" s="6"/>
+      <c r="E54" s="7"/>
+      <c r="F54" s="7"/>
       <c r="G54" s="3"/>
       <c r="H54" s="2"/>
       <c r="I54" s="2"/>
@@ -4507,9 +4501,9 @@
         <v>55</v>
       </c>
       <c r="B55" s="2"/>
-      <c r="C55" s="6"/>
+      <c r="C55" s="7"/>
       <c r="D55" s="3"/>
-      <c r="E55" s="6"/>
+      <c r="E55" s="7"/>
       <c r="F55" s="2" t="s">
         <v>56</v>
       </c>
@@ -4524,11 +4518,11 @@
       <c r="O55" s="3"/>
     </row>
     <row x14ac:dyDescent="0.25" r="56" customHeight="1" ht="18.75">
-      <c r="A56" s="6"/>
+      <c r="A56" s="7"/>
       <c r="B56" s="2"/>
-      <c r="C56" s="6"/>
+      <c r="C56" s="7"/>
       <c r="D56" s="3"/>
-      <c r="E56" s="6"/>
+      <c r="E56" s="7"/>
       <c r="F56" s="2" t="s">
         <v>57</v>
       </c>
@@ -4543,11 +4537,11 @@
       <c r="O56" s="3"/>
     </row>
     <row x14ac:dyDescent="0.25" r="57" customHeight="1" ht="18.75">
-      <c r="A57" s="6"/>
+      <c r="A57" s="7"/>
       <c r="B57" s="2"/>
-      <c r="C57" s="6"/>
+      <c r="C57" s="7"/>
       <c r="D57" s="3"/>
-      <c r="E57" s="6"/>
+      <c r="E57" s="7"/>
       <c r="F57" s="2" t="s">
         <v>58</v>
       </c>
@@ -4564,9 +4558,9 @@
     <row x14ac:dyDescent="0.25" r="58" customHeight="1" ht="18.75">
       <c r="A58" s="15"/>
       <c r="B58" s="2"/>
-      <c r="C58" s="6"/>
+      <c r="C58" s="7"/>
       <c r="D58" s="3"/>
-      <c r="E58" s="6"/>
+      <c r="E58" s="7"/>
       <c r="F58" s="15"/>
       <c r="G58" s="3"/>
       <c r="H58" s="2"/>
@@ -4583,9 +4577,9 @@
         <v>59</v>
       </c>
       <c r="B59" s="2"/>
-      <c r="C59" s="6"/>
+      <c r="C59" s="7"/>
       <c r="D59" s="3"/>
-      <c r="E59" s="6"/>
+      <c r="E59" s="7"/>
       <c r="F59" s="2"/>
       <c r="G59" s="3"/>
       <c r="H59" s="2"/>
@@ -4602,9 +4596,9 @@
         <v>60</v>
       </c>
       <c r="B60" s="2"/>
-      <c r="C60" s="6"/>
+      <c r="C60" s="7"/>
       <c r="D60" s="3"/>
-      <c r="E60" s="6"/>
+      <c r="E60" s="7"/>
       <c r="F60" s="2" t="s">
         <v>61</v>
       </c>
@@ -4619,12 +4613,12 @@
       <c r="O60" s="3"/>
     </row>
     <row x14ac:dyDescent="0.25" r="61" customHeight="1" ht="18.75">
-      <c r="A61" s="6"/>
+      <c r="A61" s="7"/>
       <c r="B61" s="2"/>
-      <c r="C61" s="6"/>
+      <c r="C61" s="7"/>
       <c r="D61" s="3"/>
-      <c r="E61" s="6"/>
-      <c r="F61" s="6"/>
+      <c r="E61" s="7"/>
+      <c r="F61" s="7"/>
       <c r="G61" s="3"/>
       <c r="H61" s="2"/>
       <c r="I61" s="2"/>
@@ -4640,9 +4634,9 @@
         <v>62</v>
       </c>
       <c r="B62" s="2"/>
-      <c r="C62" s="6"/>
+      <c r="C62" s="7"/>
       <c r="D62" s="3"/>
-      <c r="E62" s="6"/>
+      <c r="E62" s="7"/>
       <c r="F62" s="2" t="s">
         <v>63</v>
       </c>
@@ -4657,12 +4651,12 @@
       <c r="O62" s="3"/>
     </row>
     <row x14ac:dyDescent="0.25" r="63" customHeight="1" ht="18.75">
-      <c r="A63" s="6"/>
+      <c r="A63" s="7"/>
       <c r="B63" s="2"/>
-      <c r="C63" s="6"/>
+      <c r="C63" s="7"/>
       <c r="D63" s="3"/>
-      <c r="E63" s="6"/>
-      <c r="F63" s="6"/>
+      <c r="E63" s="7"/>
+      <c r="F63" s="7"/>
       <c r="G63" s="3"/>
       <c r="H63" s="2"/>
       <c r="I63" s="2"/>
@@ -4678,9 +4672,9 @@
         <v>64</v>
       </c>
       <c r="B64" s="2"/>
-      <c r="C64" s="6"/>
+      <c r="C64" s="7"/>
       <c r="D64" s="3"/>
-      <c r="E64" s="6"/>
+      <c r="E64" s="7"/>
       <c r="F64" s="2" t="s">
         <v>65</v>
       </c>
@@ -4697,9 +4691,9 @@
     <row x14ac:dyDescent="0.25" r="65" customHeight="1" ht="18.75">
       <c r="A65" s="2"/>
       <c r="B65" s="2"/>
-      <c r="C65" s="6"/>
+      <c r="C65" s="7"/>
       <c r="D65" s="3"/>
-      <c r="E65" s="6"/>
+      <c r="E65" s="7"/>
       <c r="F65" s="2" t="s">
         <v>66</v>
       </c>
@@ -4714,12 +4708,12 @@
       <c r="O65" s="3"/>
     </row>
     <row x14ac:dyDescent="0.25" r="66" customHeight="1" ht="18.75">
-      <c r="A66" s="6"/>
+      <c r="A66" s="7"/>
       <c r="B66" s="2"/>
-      <c r="C66" s="6"/>
+      <c r="C66" s="7"/>
       <c r="D66" s="3"/>
-      <c r="E66" s="6"/>
-      <c r="F66" s="6"/>
+      <c r="E66" s="7"/>
+      <c r="F66" s="7"/>
       <c r="G66" s="3"/>
       <c r="H66" s="2"/>
       <c r="I66" s="2"/>
@@ -4752,7 +4746,7 @@
       <c r="O67" s="3"/>
     </row>
     <row x14ac:dyDescent="0.25" r="68" customHeight="1" ht="18.75">
-      <c r="A68" s="6"/>
+      <c r="A68" s="7"/>
       <c r="B68" s="2"/>
       <c r="C68" s="2"/>
       <c r="D68" s="3"/>
@@ -4771,7 +4765,7 @@
       <c r="O68" s="3"/>
     </row>
     <row x14ac:dyDescent="0.25" r="69" customHeight="1" ht="18.75">
-      <c r="A69" s="6"/>
+      <c r="A69" s="7"/>
       <c r="B69" s="2"/>
       <c r="C69" s="2"/>
       <c r="D69" s="3"/>
@@ -4809,7 +4803,7 @@
       <c r="O70" s="3"/>
     </row>
     <row x14ac:dyDescent="0.25" r="71" customHeight="1" ht="18.75">
-      <c r="A71" s="6"/>
+      <c r="A71" s="7"/>
       <c r="B71" s="2"/>
       <c r="C71" s="2"/>
       <c r="D71" s="3"/>
@@ -4828,7 +4822,7 @@
       <c r="O71" s="3"/>
     </row>
     <row x14ac:dyDescent="0.25" r="72" customHeight="1" ht="18.75">
-      <c r="A72" s="6"/>
+      <c r="A72" s="7"/>
       <c r="B72" s="2"/>
       <c r="C72" s="2"/>
       <c r="D72" s="3"/>
@@ -4845,7 +4839,7 @@
       <c r="O72" s="3"/>
     </row>
     <row x14ac:dyDescent="0.25" r="73" customHeight="1" ht="18.75">
-      <c r="A73" s="6"/>
+      <c r="A73" s="7"/>
       <c r="B73" s="2"/>
       <c r="C73" s="2"/>
       <c r="D73" s="3"/>
@@ -4864,79 +4858,79 @@
       <c r="O73" s="3"/>
     </row>
     <row x14ac:dyDescent="0.25" r="74" customHeight="1" ht="18.75">
-      <c r="A74" s="3"/>
-      <c r="B74" s="6"/>
+      <c r="A74" s="6"/>
+      <c r="B74" s="7"/>
       <c r="C74" s="2"/>
-      <c r="D74" s="6"/>
-      <c r="E74" s="6"/>
+      <c r="D74" s="7"/>
+      <c r="E74" s="7"/>
       <c r="F74" s="2"/>
       <c r="G74" s="2"/>
       <c r="H74" s="2"/>
       <c r="I74" s="2"/>
-      <c r="J74" s="7"/>
-      <c r="K74" s="3"/>
+      <c r="J74" s="8"/>
+      <c r="K74" s="6"/>
       <c r="L74" s="13"/>
       <c r="M74" s="3"/>
       <c r="N74" s="3"/>
       <c r="O74" s="3"/>
     </row>
     <row x14ac:dyDescent="0.25" r="75" customHeight="1" ht="18.75">
-      <c r="A75" s="3"/>
+      <c r="A75" s="6"/>
       <c r="B75" s="2" t="s">
         <v>73</v>
       </c>
       <c r="C75" s="2" t="s">
         <v>74</v>
       </c>
-      <c r="D75" s="6"/>
-      <c r="E75" s="6"/>
+      <c r="D75" s="7"/>
+      <c r="E75" s="7"/>
       <c r="F75" s="2"/>
       <c r="G75" s="2"/>
       <c r="H75" s="2"/>
       <c r="I75" s="2"/>
-      <c r="J75" s="7"/>
-      <c r="K75" s="3"/>
+      <c r="J75" s="8"/>
+      <c r="K75" s="6"/>
       <c r="L75" s="13"/>
       <c r="M75" s="3"/>
       <c r="N75" s="3"/>
       <c r="O75" s="3"/>
     </row>
     <row x14ac:dyDescent="0.25" r="76" customHeight="1" ht="18.75">
-      <c r="A76" s="3"/>
+      <c r="A76" s="6"/>
       <c r="B76" s="2"/>
       <c r="C76" s="2" t="s">
         <v>75</v>
       </c>
-      <c r="D76" s="6"/>
-      <c r="E76" s="6"/>
+      <c r="D76" s="7"/>
+      <c r="E76" s="7"/>
       <c r="F76" s="2"/>
       <c r="G76" s="2"/>
       <c r="H76" s="2"/>
       <c r="I76" s="2"/>
-      <c r="J76" s="7"/>
-      <c r="K76" s="3"/>
+      <c r="J76" s="8"/>
+      <c r="K76" s="6"/>
       <c r="L76" s="13"/>
       <c r="M76" s="3"/>
       <c r="N76" s="3"/>
       <c r="O76" s="3"/>
     </row>
     <row x14ac:dyDescent="0.25" r="77" customHeight="1" ht="18.75">
-      <c r="A77" s="3"/>
-      <c r="B77" s="7" t="s">
+      <c r="A77" s="6"/>
+      <c r="B77" s="8" t="s">
         <v>76</v>
       </c>
       <c r="C77" s="2" t="s">
         <v>77</v>
       </c>
-      <c r="D77" s="7"/>
-      <c r="E77" s="3"/>
-      <c r="F77" s="3"/>
+      <c r="D77" s="8"/>
+      <c r="E77" s="6"/>
+      <c r="F77" s="6"/>
       <c r="G77" s="3"/>
       <c r="H77" s="2"/>
       <c r="I77" s="2"/>
-      <c r="J77" s="3"/>
-      <c r="K77" s="3"/>
-      <c r="L77" s="3"/>
+      <c r="J77" s="6"/>
+      <c r="K77" s="6"/>
+      <c r="L77" s="6"/>
       <c r="M77" s="3"/>
       <c r="N77" s="3"/>
       <c r="O77" s="3"/>
@@ -4965,14 +4959,14 @@
       <c r="B79" s="2"/>
       <c r="C79" s="2"/>
       <c r="D79" s="3"/>
-      <c r="E79" s="3"/>
+      <c r="E79" s="6"/>
       <c r="F79" s="2"/>
       <c r="G79" s="3"/>
-      <c r="H79" s="3"/>
-      <c r="I79" s="3"/>
-      <c r="J79" s="7"/>
-      <c r="K79" s="7"/>
-      <c r="L79" s="3"/>
+      <c r="H79" s="6"/>
+      <c r="I79" s="6"/>
+      <c r="J79" s="8"/>
+      <c r="K79" s="8"/>
+      <c r="L79" s="6"/>
       <c r="M79" s="3"/>
       <c r="N79" s="3"/>
       <c r="O79" s="2"/>
@@ -4984,14 +4978,14 @@
       <c r="B80" s="2"/>
       <c r="C80" s="2"/>
       <c r="D80" s="3"/>
-      <c r="E80" s="3"/>
+      <c r="E80" s="6"/>
       <c r="F80" s="2"/>
       <c r="G80" s="3"/>
-      <c r="H80" s="3"/>
-      <c r="I80" s="3"/>
-      <c r="J80" s="7"/>
-      <c r="K80" s="7"/>
-      <c r="L80" s="3"/>
+      <c r="H80" s="6"/>
+      <c r="I80" s="6"/>
+      <c r="J80" s="8"/>
+      <c r="K80" s="8"/>
+      <c r="L80" s="6"/>
       <c r="M80" s="3"/>
       <c r="N80" s="3"/>
       <c r="O80" s="2"/>

</xml_diff>